<commit_message>
, added some distribution formulas
</commit_message>
<xml_diff>
--- a/investing/africatop250_dfs/africa_top250.xlsx
+++ b/investing/africatop250_dfs/africa_top250.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M.Seidel\PycharmProjects\safe_haven_investing\investing\africatop250_dfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6756D5C6-E4C0-4DC8-AB5F-93C0A2E7EA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C60925-0D0B-4459-8EE4-C524394B0443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A5AF3B39-A7EE-46F6-9BC6-CCBBABD8CBFE}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$K$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$C$1:$C$251</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="424">
   <si>
     <t>Naspers</t>
   </si>
@@ -896,9 +896,6 @@
     <t>−10</t>
   </si>
   <si>
-    <t>Egyptian International Tourism Projects</t>
-  </si>
-  <si>
     <t>I&amp;M Holdings</t>
   </si>
   <si>
@@ -1164,13 +1161,163 @@
   </si>
   <si>
     <t>MTH.JO</t>
+  </si>
+  <si>
+    <t>EGS39061C014.CA</t>
+  </si>
+  <si>
+    <t>KST.JO</t>
+  </si>
+  <si>
+    <t>EU4.F</t>
+  </si>
+  <si>
+    <t>N8C.BE</t>
+  </si>
+  <si>
+    <t>CML.JO</t>
+  </si>
+  <si>
+    <t>TUWOY</t>
+  </si>
+  <si>
+    <t>TUWLF</t>
+  </si>
+  <si>
+    <t>EGS745L1C014.CA</t>
+  </si>
+  <si>
+    <t>KRO.JO</t>
+  </si>
+  <si>
+    <t>OMN.JO</t>
+  </si>
+  <si>
+    <t>TSG.JO</t>
+  </si>
+  <si>
+    <t>G5E.F</t>
+  </si>
+  <si>
+    <t>EGS42111C012.CA</t>
+  </si>
+  <si>
+    <t>KAP.JO</t>
+  </si>
+  <si>
+    <t>AFE.JO</t>
+  </si>
+  <si>
+    <t>A7Z.F</t>
+  </si>
+  <si>
+    <t>drd</t>
+  </si>
+  <si>
+    <t>RCL.JO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>ACL.JO</t>
+  </si>
+  <si>
+    <t>SGHC</t>
+  </si>
+  <si>
+    <t>SPG.JO</t>
+  </si>
+  <si>
+    <t>siehe Group</t>
+  </si>
+  <si>
+    <t>EGS673Y1C015.CA</t>
+  </si>
+  <si>
+    <t>AFT.JO</t>
+  </si>
+  <si>
+    <t>HCI.JO</t>
+  </si>
+  <si>
+    <t>ADH.JO</t>
+  </si>
+  <si>
+    <t>JSEJF</t>
+  </si>
+  <si>
+    <t>JSE.JO</t>
+  </si>
+  <si>
+    <t>AIP.JO</t>
+  </si>
+  <si>
+    <t>DTTLY</t>
+  </si>
+  <si>
+    <t>DTC.JO</t>
+  </si>
+  <si>
+    <t>EGS3D041C017.CA</t>
+  </si>
+  <si>
+    <t>SHG.JO</t>
+  </si>
+  <si>
+    <t>EGS305I1C011.CA</t>
+  </si>
+  <si>
+    <t>DYLLF</t>
+  </si>
+  <si>
+    <t>EGS380S1C017.CA</t>
+  </si>
+  <si>
+    <t>EGS70011C019-EGP.CA</t>
+  </si>
+  <si>
+    <t>Egyptian International Tourism</t>
+  </si>
+  <si>
+    <t>LBR.JO</t>
+  </si>
+  <si>
+    <t>RZT.F</t>
+  </si>
+  <si>
+    <t>MRF.JO</t>
+  </si>
+  <si>
+    <t>GRIN</t>
+  </si>
+  <si>
+    <t>GND.JO</t>
+  </si>
+  <si>
+    <t>GSH.JO</t>
+  </si>
+  <si>
+    <t>7YZ.F</t>
+  </si>
+  <si>
+    <t>THA.JO</t>
+  </si>
+  <si>
+    <t>RNRTY</t>
+  </si>
+  <si>
+    <t>EGS60171C013-EGP.CA</t>
+  </si>
+  <si>
+    <t>RY1B.F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1198,12 +1345,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1218,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -1230,6 +1383,19 @@
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1546,13 +1712,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9628B33F-28A3-4F29-8CFD-80C940AAB6C6}">
-  <dimension ref="A1:K251"/>
+  <dimension ref="A1:L251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M104" sqref="M104"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="K162" sqref="K162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
@@ -1560,39 +1726,39 @@
     <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" t="s">
         <v>302</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G1" t="s">
+        <v>298</v>
+      </c>
+      <c r="H1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I1" t="s">
+        <v>300</v>
+      </c>
+      <c r="J1" t="s">
         <v>303</v>
       </c>
-      <c r="C1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D1" t="s">
-        <v>296</v>
-      </c>
-      <c r="E1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F1" t="s">
-        <v>298</v>
-      </c>
-      <c r="G1" t="s">
-        <v>299</v>
-      </c>
-      <c r="H1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I1" t="s">
-        <v>301</v>
-      </c>
-      <c r="J1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="41.4">
+    </row>
+    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1621,10 +1787,10 @@
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="41.4">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1653,10 +1819,10 @@
         <v>4</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="27.6">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1685,10 +1851,10 @@
         <v>6</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="27.6">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1717,10 +1883,10 @@
         <v>8</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="27.6">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1749,10 +1915,10 @@
         <v>6</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="27.6">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1781,10 +1947,10 @@
         <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="27.6">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1813,10 +1979,10 @@
         <v>6</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="41.4">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1845,10 +2011,10 @@
         <v>4</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="41.4">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1877,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="41.4">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1909,10 +2075,10 @@
         <v>4</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="41.4">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1941,10 +2107,10 @@
         <v>4</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="27.6">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1973,10 +2139,10 @@
         <v>8</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="27.6">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2005,10 +2171,10 @@
         <v>8</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="41.4">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2037,10 +2203,10 @@
         <v>4</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="41.4">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2069,10 +2235,10 @@
         <v>4</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="27.6">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2101,10 +2267,10 @@
         <v>6</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="27.6">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2133,10 +2299,10 @@
         <v>6</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="27.6">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2165,10 +2331,10 @@
         <v>8</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="27.6">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2197,10 +2363,10 @@
         <v>6</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2229,10 +2395,10 @@
         <v>4</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="41.4">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2261,10 +2427,10 @@
         <v>2</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="27.6">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2293,10 +2459,10 @@
         <v>6</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2325,10 +2491,10 @@
         <v>6</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="27.6">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2357,10 +2523,10 @@
         <v>32</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="27.6">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2389,10 +2555,10 @@
         <v>8</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="27.6">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2421,10 +2587,10 @@
         <v>6</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="27.6">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2453,10 +2619,10 @@
         <v>36</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="41.4">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2485,10 +2651,10 @@
         <v>4</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="27.6">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2517,10 +2683,10 @@
         <v>39</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="27.6">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2549,10 +2715,10 @@
         <v>6</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="41.4">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2581,10 +2747,10 @@
         <v>4</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2613,10 +2779,10 @@
         <v>6</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2645,10 +2811,10 @@
         <v>6</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2677,10 +2843,10 @@
         <v>45</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="27.6">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2709,10 +2875,10 @@
         <v>39</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="41.4">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2741,10 +2907,10 @@
         <v>2</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="27.6">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2773,10 +2939,10 @@
         <v>6</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="41.4">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2805,10 +2971,10 @@
         <v>4</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="41.4">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2837,10 +3003,10 @@
         <v>4</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2869,10 +3035,10 @@
         <v>6</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="41.4">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2901,10 +3067,10 @@
         <v>4</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="27.6">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2933,10 +3099,10 @@
         <v>6</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2965,10 +3131,10 @@
         <v>2</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="27.6">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2997,10 +3163,10 @@
         <v>8</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="41.4">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3029,10 +3195,10 @@
         <v>2</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="27.6">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3061,10 +3227,10 @@
         <v>6</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3093,10 +3259,10 @@
         <v>8</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3125,10 +3291,10 @@
         <v>6</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="27.6">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3157,10 +3323,10 @@
         <v>39</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="41.4">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3189,10 +3355,10 @@
         <v>4</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="41.4">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3221,10 +3387,10 @@
         <v>4</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="41.4">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3253,10 +3419,10 @@
         <v>6</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="27.6">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3285,10 +3451,10 @@
         <v>6</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="41.4">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3317,10 +3483,10 @@
         <v>4</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3349,10 +3515,10 @@
         <v>8</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3381,10 +3547,10 @@
         <v>2</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3413,13 +3579,13 @@
         <v>2</v>
       </c>
       <c r="J58" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="K58" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="K58" s="4" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="27.6">
+    </row>
+    <row r="59" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3448,10 +3614,10 @@
         <v>79</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3480,10 +3646,10 @@
         <v>2</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3512,10 +3678,10 @@
         <v>6</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="41.4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3544,10 +3710,10 @@
         <v>2</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3576,10 +3742,10 @@
         <v>36</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="27.6">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3608,10 +3774,10 @@
         <v>39</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3640,10 +3806,10 @@
         <v>6</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="41.4">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3672,10 +3838,10 @@
         <v>2</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="41.4">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3704,10 +3870,10 @@
         <v>2</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="41.4">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3736,10 +3902,10 @@
         <v>4</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="41.4">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3768,10 +3934,10 @@
         <v>2</v>
       </c>
       <c r="J69" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3800,10 +3966,10 @@
         <v>6</v>
       </c>
       <c r="J70" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -3832,10 +3998,10 @@
         <v>2</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="41.4">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -3864,10 +4030,10 @@
         <v>4</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -3896,10 +4062,10 @@
         <v>94</v>
       </c>
       <c r="J73" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3928,10 +4094,10 @@
         <v>2</v>
       </c>
       <c r="J74" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" ht="27.6">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3960,10 +4126,10 @@
         <v>6</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" ht="27.6">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3992,10 +4158,10 @@
         <v>6</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4024,10 +4190,10 @@
         <v>8</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4056,10 +4222,10 @@
         <v>6</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="41.4">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4088,10 +4254,10 @@
         <v>4</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" ht="27.6">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4120,13 +4286,13 @@
         <v>45</v>
       </c>
       <c r="J80" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="K80" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="K80" s="3" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="27.6">
+    </row>
+    <row r="81" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4155,10 +4321,10 @@
         <v>45</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4187,10 +4353,10 @@
         <v>6</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4219,10 +4385,10 @@
         <v>39</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="41.4">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4251,10 +4417,10 @@
         <v>2</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4283,10 +4449,10 @@
         <v>6</v>
       </c>
       <c r="J85" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4315,10 +4481,10 @@
         <v>8</v>
       </c>
       <c r="J86" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="27.6">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4347,10 +4513,10 @@
         <v>94</v>
       </c>
       <c r="J87" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="27.6">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4379,10 +4545,10 @@
         <v>36</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="27.6">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4411,10 +4577,10 @@
         <v>6</v>
       </c>
       <c r="J89" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="27.6">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4443,10 +4609,10 @@
         <v>39</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4475,10 +4641,10 @@
         <v>8</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="41.4">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4507,10 +4673,10 @@
         <v>6</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4539,10 +4705,10 @@
         <v>39</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="41.4">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4571,10 +4737,10 @@
         <v>2</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="27.6">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4603,10 +4769,10 @@
         <v>6</v>
       </c>
       <c r="J95" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="55.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4635,10 +4801,10 @@
         <v>2</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4667,10 +4833,10 @@
         <v>6</v>
       </c>
       <c r="J97" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="41.4">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4699,10 +4865,10 @@
         <v>2</v>
       </c>
       <c r="J98" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4731,10 +4897,10 @@
         <v>2</v>
       </c>
       <c r="J99" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="27.6">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4763,10 +4929,10 @@
         <v>39</v>
       </c>
       <c r="J100" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="27.6">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4795,10 +4961,10 @@
         <v>6</v>
       </c>
       <c r="J101" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="41.4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4826,8 +4992,13 @@
       <c r="I102" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:10">
+      <c r="J102" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -4855,8 +5026,13 @@
       <c r="I103" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" ht="41.4">
+      <c r="J103" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+    </row>
+    <row r="104" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -4884,8 +5060,13 @@
       <c r="I104" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" ht="27.6">
+      <c r="J104" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+    </row>
+    <row r="105" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -4913,8 +5094,15 @@
       <c r="I105" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" ht="27.6">
+      <c r="J105" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="L105" s="2"/>
+    </row>
+    <row r="106" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -4942,8 +5130,13 @@
       <c r="I106" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="27.6">
+      <c r="J106" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K106" s="2"/>
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -4971,8 +5164,13 @@
       <c r="I107" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="27.6">
+      <c r="J107" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K107" s="2"/>
+      <c r="L107" s="2"/>
+    </row>
+    <row r="108" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -5000,8 +5198,15 @@
       <c r="I108" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="109" spans="1:10">
+      <c r="J108" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="L108" s="2"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -5029,8 +5234,13 @@
       <c r="I109" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" ht="27.6">
+      <c r="J109" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K109" s="2"/>
+      <c r="L109" s="2"/>
+    </row>
+    <row r="110" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -5058,8 +5268,13 @@
       <c r="I110" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="41.4">
+      <c r="J110" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K110" s="2"/>
+      <c r="L110" s="2"/>
+    </row>
+    <row r="111" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -5087,8 +5302,13 @@
       <c r="I111" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:10">
+      <c r="J111" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -5116,8 +5336,15 @@
       <c r="I112" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="27.6">
+      <c r="J112" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="K112" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="L112" s="2"/>
+    </row>
+    <row r="113" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -5145,8 +5372,13 @@
       <c r="I113" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="27.6">
+      <c r="J113" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+    </row>
+    <row r="114" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -5174,8 +5406,13 @@
       <c r="I114" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="115" spans="1:9">
+      <c r="J114" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -5203,8 +5440,13 @@
       <c r="I115" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="27.6">
+      <c r="J115" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+    </row>
+    <row r="116" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -5232,8 +5474,13 @@
       <c r="I116" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="117" spans="1:9">
+      <c r="J116" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -5261,8 +5508,13 @@
       <c r="I117" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="41.4">
+      <c r="J117" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+    </row>
+    <row r="118" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -5290,8 +5542,13 @@
       <c r="I118" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="41.4">
+      <c r="J118" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+    </row>
+    <row r="119" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -5317,8 +5574,13 @@
       <c r="I119" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="41.4">
+      <c r="J119" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="K119" s="2"/>
+      <c r="L119" s="2"/>
+    </row>
+    <row r="120" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -5346,8 +5608,13 @@
       <c r="I120" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="27.6">
+      <c r="J120" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+    </row>
+    <row r="121" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -5375,8 +5642,13 @@
       <c r="I121" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="41.4">
+      <c r="J121" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+    </row>
+    <row r="122" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -5404,8 +5676,13 @@
       <c r="I122" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="27.6">
+      <c r="J122" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+    </row>
+    <row r="123" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -5433,8 +5710,15 @@
       <c r="I123" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="41.4">
+      <c r="J123" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L123" s="2"/>
+    </row>
+    <row r="124" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -5462,8 +5746,13 @@
       <c r="I124" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="41.4">
+      <c r="J124" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2"/>
+    </row>
+    <row r="125" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -5491,8 +5780,13 @@
       <c r="I125" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="41.4">
+      <c r="J125" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2"/>
+    </row>
+    <row r="126" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -5520,8 +5814,13 @@
       <c r="I126" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="41.4">
+      <c r="J126" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="K126" s="2"/>
+      <c r="L126" s="2"/>
+    </row>
+    <row r="127" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -5549,8 +5848,15 @@
       <c r="I127" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="27.6">
+      <c r="J127" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="K127" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="L127" s="2"/>
+    </row>
+    <row r="128" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -5578,8 +5884,13 @@
       <c r="I128" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="129" spans="1:9">
+      <c r="J128" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K128" s="2"/>
+      <c r="L128" s="2"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -5607,8 +5918,13 @@
       <c r="I129" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="27.6">
+      <c r="J129" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K129" s="2"/>
+      <c r="L129" s="2"/>
+    </row>
+    <row r="130" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -5636,8 +5952,13 @@
       <c r="I130" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" ht="41.4">
+      <c r="J130" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K130" s="2"/>
+      <c r="L130" s="2"/>
+    </row>
+    <row r="131" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -5665,8 +5986,13 @@
       <c r="I131" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" ht="41.4">
+      <c r="J131" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K131" s="2"/>
+      <c r="L131" s="2"/>
+    </row>
+    <row r="132" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -5694,8 +6020,13 @@
       <c r="I132" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" ht="41.4">
+      <c r="J132" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K132" s="2"/>
+      <c r="L132" s="2"/>
+    </row>
+    <row r="133" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -5723,8 +6054,13 @@
       <c r="I133" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" ht="27.6">
+      <c r="J133" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K133" s="2"/>
+      <c r="L133" s="2"/>
+    </row>
+    <row r="134" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -5752,8 +6088,13 @@
       <c r="I134" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" ht="55.2">
+      <c r="J134" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K134" s="2"/>
+      <c r="L134" s="2"/>
+    </row>
+    <row r="135" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -5781,8 +6122,13 @@
       <c r="I135" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" ht="41.4">
+      <c r="J135" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K135" s="2"/>
+      <c r="L135" s="2"/>
+    </row>
+    <row r="136" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -5810,8 +6156,13 @@
       <c r="I136" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" ht="41.4">
+      <c r="J136" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="K136" s="2"/>
+      <c r="L136" s="2"/>
+    </row>
+    <row r="137" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -5839,8 +6190,13 @@
       <c r="I137" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" ht="41.4">
+      <c r="J137" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="K137" s="2"/>
+      <c r="L137" s="2"/>
+    </row>
+    <row r="138" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -5868,8 +6224,15 @@
       <c r="I138" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" ht="27.6">
+      <c r="J138" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="K138" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="L138" s="2"/>
+    </row>
+    <row r="139" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -5897,37 +6260,47 @@
       <c r="I139" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" ht="27.6">
-      <c r="A140" s="1">
+      <c r="J139" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="K139" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="L139" s="2"/>
+    </row>
+    <row r="140" spans="1:12" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A140" s="5">
         <v>139</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B140" s="6">
         <v>123</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="D140" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E140" s="3">
+      <c r="E140" s="7">
         <v>743</v>
       </c>
-      <c r="F140" s="3">
+      <c r="F140" s="7">
         <v>744</v>
       </c>
-      <c r="G140" s="3">
+      <c r="G140" s="7">
         <v>420</v>
       </c>
-      <c r="H140" s="3" t="s">
+      <c r="H140" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="I140" s="2" t="s">
+      <c r="I140" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" ht="41.4">
+      <c r="J140" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -5955,8 +6328,11 @@
       <c r="I141" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" ht="27.6">
+      <c r="J141" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -5984,8 +6360,11 @@
       <c r="I142" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" ht="27.6">
+      <c r="J142" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -6013,8 +6392,11 @@
       <c r="I143" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" ht="41.4">
+      <c r="J143" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -6042,8 +6424,11 @@
       <c r="I144" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" ht="41.4">
+      <c r="J144" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -6071,8 +6456,11 @@
       <c r="I145" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" ht="41.4">
+      <c r="J145" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -6100,8 +6488,11 @@
       <c r="I146" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" ht="41.4">
+      <c r="J146" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -6129,8 +6520,11 @@
       <c r="I147" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" ht="27.6">
+      <c r="J147" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -6158,8 +6552,11 @@
       <c r="I148" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" ht="41.4">
+      <c r="J148" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -6187,8 +6584,11 @@
       <c r="I149" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" ht="27.6">
+      <c r="J149" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -6216,8 +6616,14 @@
       <c r="I150" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" ht="27.6">
+      <c r="J150" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="K150" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -6245,8 +6651,11 @@
       <c r="I151" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" ht="41.4">
+      <c r="J151" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -6274,8 +6683,11 @@
       <c r="I152" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" ht="27.6">
+      <c r="J152" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -6303,8 +6715,11 @@
       <c r="I153" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" ht="27.6">
+      <c r="J153" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -6332,8 +6747,11 @@
       <c r="I154" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" ht="27.6">
+      <c r="J154" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -6361,8 +6779,11 @@
       <c r="I155" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" ht="41.4">
+      <c r="J155" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -6390,8 +6811,11 @@
       <c r="I156" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" ht="27.6">
+      <c r="J156" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -6419,8 +6843,11 @@
       <c r="I157" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="158" spans="1:9">
+      <c r="J157" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -6448,8 +6875,11 @@
       <c r="I158" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" ht="27.6">
+      <c r="J158" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -6477,8 +6907,11 @@
       <c r="I159" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" ht="41.4">
+      <c r="J159" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -6506,8 +6939,11 @@
       <c r="I160" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" ht="27.6">
+      <c r="J160" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -6535,8 +6971,11 @@
       <c r="I161" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" ht="41.4">
+      <c r="J161" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -6564,8 +7003,14 @@
       <c r="I162" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" ht="27.6">
+      <c r="J162" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="K162" s="4" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -6593,8 +7038,11 @@
       <c r="I163" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" ht="27.6">
+      <c r="J163" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -6622,8 +7070,11 @@
       <c r="I164" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" ht="27.6">
+      <c r="J164" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -6651,8 +7102,11 @@
       <c r="I165" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" ht="27.6">
+      <c r="J165" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -6680,8 +7134,11 @@
       <c r="I166" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" ht="27.6">
+      <c r="J166" s="4" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -6709,8 +7166,11 @@
       <c r="I167" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" ht="27.6">
+      <c r="J167" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -6738,8 +7198,11 @@
       <c r="I168" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" ht="27.6">
+      <c r="J168" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -6767,8 +7230,11 @@
       <c r="I169" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="170" spans="1:9">
+      <c r="J169" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -6796,8 +7262,11 @@
       <c r="I170" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" ht="41.4">
+      <c r="J170" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -6825,8 +7294,11 @@
       <c r="I171" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" ht="41.4">
+      <c r="J171" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -6855,7 +7327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="27.6">
+    <row r="173" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -6884,7 +7356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="41.4">
+    <row r="174" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -6913,7 +7385,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="27.6">
+    <row r="175" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -6942,7 +7414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="27.6">
+    <row r="176" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -6971,7 +7443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="27.6">
+    <row r="177" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -7000,7 +7472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="41.4">
+    <row r="178" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -7029,7 +7501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="41.4">
+    <row r="179" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -7058,7 +7530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:9">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -7087,7 +7559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="27.6">
+    <row r="181" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -7116,7 +7588,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="182" spans="1:9" ht="41.4">
+    <row r="182" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -7145,7 +7617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:9" ht="27.6">
+    <row r="183" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -7174,7 +7646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:9" ht="27.6">
+    <row r="184" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -7203,7 +7675,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="27.6">
+    <row r="185" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -7232,7 +7704,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="186" spans="1:9" ht="41.4">
+    <row r="186" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -7261,7 +7733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:9" ht="41.4">
+    <row r="187" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -7290,7 +7762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:9">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -7319,7 +7791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="27.6">
+    <row r="189" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -7348,7 +7820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="55.2">
+    <row r="190" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -7377,7 +7849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="41.4">
+    <row r="191" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -7406,7 +7878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="41.4">
+    <row r="192" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -7435,7 +7907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="41.4">
+    <row r="193" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -7464,7 +7936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="27.6">
+    <row r="194" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -7493,7 +7965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="27.6">
+    <row r="195" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -7522,7 +7994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="27.6">
+    <row r="196" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -7551,7 +8023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="27.6">
+    <row r="197" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -7580,7 +8052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="198" spans="1:9" ht="27.6">
+    <row r="198" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -7609,7 +8081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="27.6">
+    <row r="199" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -7638,7 +8110,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:9" ht="41.4">
+    <row r="200" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -7667,7 +8139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -7696,7 +8168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:9" ht="41.4">
+    <row r="202" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -7725,7 +8197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="27.6">
+    <row r="203" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -7754,7 +8226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -7783,7 +8255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:9" ht="41.4">
+    <row r="205" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -7812,7 +8284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:9" ht="27.6">
+    <row r="206" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -7841,7 +8313,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="41.4">
+    <row r="207" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -7870,7 +8342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:9" ht="27.6">
+    <row r="208" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -7899,7 +8371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="27.6">
+    <row r="209" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -7928,7 +8400,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="210" spans="1:9" ht="27.6">
+    <row r="210" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -7957,7 +8429,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="41.4">
+    <row r="211" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -7986,7 +8458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="41.4">
+    <row r="212" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -8015,7 +8487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -8044,7 +8516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:9" ht="27.6">
+    <row r="214" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -8073,7 +8545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="215" spans="1:9" ht="27.6">
+    <row r="215" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -8102,7 +8574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:9" ht="27.6">
+    <row r="216" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -8131,7 +8603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -8160,7 +8632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:9" ht="27.6">
+    <row r="218" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -8189,7 +8661,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="219" spans="1:9" ht="27.6">
+    <row r="219" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -8218,7 +8690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="220" spans="1:9" ht="41.4">
+    <row r="220" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -8247,7 +8719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="27.6">
+    <row r="221" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -8276,7 +8748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="27.6">
+    <row r="222" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -8305,7 +8777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="27.6">
+    <row r="223" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -8334,7 +8806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:9" ht="27.6">
+    <row r="224" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -8363,7 +8835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="225" spans="1:9" ht="41.4">
+    <row r="225" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -8392,7 +8864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:9" ht="27.6">
+    <row r="226" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -8421,7 +8893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="227" spans="1:9" ht="27.6">
+    <row r="227" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -8450,7 +8922,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="228" spans="1:9" ht="27.6">
+    <row r="228" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -8479,7 +8951,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="229" spans="1:9" ht="41.4">
+    <row r="229" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -8508,7 +8980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:9" ht="41.4">
+    <row r="230" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -8537,7 +9009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:9" ht="27.6">
+    <row r="231" spans="1:12" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -8565,8 +9037,17 @@
       <c r="I231" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="232" spans="1:9" ht="41.4">
+      <c r="J231" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="K231" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="L231" s="9" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -8594,8 +9075,11 @@
       <c r="I232" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="233" spans="1:9" ht="41.4">
+      <c r="J232" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -8623,8 +9107,11 @@
       <c r="I233" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="234" spans="1:9" ht="41.4">
+      <c r="J233" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -8652,8 +9139,11 @@
       <c r="I234" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="235" spans="1:9" ht="41.4">
+      <c r="J234" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -8681,8 +9171,14 @@
       <c r="I235" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="236" spans="1:9" ht="41.4">
+      <c r="J235" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="K235" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -8710,8 +9206,11 @@
       <c r="I236" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="237" spans="1:9" ht="27.6">
+      <c r="J236" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -8739,8 +9238,11 @@
       <c r="I237" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="238" spans="1:9" ht="41.4">
+      <c r="J237" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="238" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -8768,8 +9270,11 @@
       <c r="I238" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="239" spans="1:9" ht="41.4">
+      <c r="J238" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -8797,8 +9302,11 @@
       <c r="I239" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="240" spans="1:9" ht="41.4">
+      <c r="J239" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -8826,8 +9334,11 @@
       <c r="I240" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" ht="27.6">
+      <c r="J240" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -8855,8 +9366,11 @@
       <c r="I241" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="242" spans="1:9" ht="41.4">
+      <c r="J241" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -8864,7 +9378,7 @@
         <v>60</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>285</v>
+        <v>412</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>49</v>
@@ -8884,8 +9398,11 @@
       <c r="I242" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="243" spans="1:9">
+      <c r="J242" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -8893,7 +9410,7 @@
         <v>198</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D243" s="2" t="s">
         <v>17</v>
@@ -8913,8 +9430,11 @@
       <c r="I243" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="244" spans="1:9" ht="41.4">
+      <c r="J243" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -8922,7 +9442,7 @@
         <v>216</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D244" s="2" t="s">
         <v>49</v>
@@ -8942,8 +9462,11 @@
       <c r="I244" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="245" spans="1:9" ht="41.4">
+      <c r="J244" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -8951,7 +9474,7 @@
         <v>60</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D245" s="2" t="s">
         <v>19</v>
@@ -8971,8 +9494,11 @@
       <c r="I245" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="246" spans="1:9" ht="27.6">
+      <c r="J245" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -8980,7 +9506,7 @@
         <v>60</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D246" s="2" t="s">
         <v>62</v>
@@ -9000,8 +9526,11 @@
       <c r="I246" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="247" spans="1:9" ht="27.6">
+      <c r="J246" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -9009,7 +9538,7 @@
         <v>60</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D247" s="2" t="s">
         <v>51</v>
@@ -9029,8 +9558,11 @@
       <c r="I247" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="248" spans="1:9" ht="41.4">
+      <c r="J247" s="4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -9038,7 +9570,7 @@
         <v>193</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D248" s="2" t="s">
         <v>49</v>
@@ -9058,8 +9590,11 @@
       <c r="I248" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="249" spans="1:9" ht="27.6">
+      <c r="J248" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -9067,7 +9602,7 @@
         <v>60</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D249" s="2" t="s">
         <v>1</v>
@@ -9087,8 +9622,11 @@
       <c r="I249" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="250" spans="1:9" ht="41.4">
+      <c r="J249" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -9096,7 +9634,7 @@
         <v>234</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D250" s="2" t="s">
         <v>120</v>
@@ -9116,8 +9654,11 @@
       <c r="I250" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="251" spans="1:9" ht="41.4">
+      <c r="J250" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -9125,7 +9666,7 @@
         <v>231</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D251" s="2" t="s">
         <v>1</v>
@@ -9145,9 +9686,12 @@
       <c r="I251" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="J251" s="4" t="s">
+        <v>407</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K251" xr:uid="{9628B33F-28A3-4F29-8CFD-80C940AAB6C6}"/>
+  <autoFilter ref="C1:C251" xr:uid="{9628B33F-28A3-4F29-8CFD-80C940AAB6C6}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>